<commit_message>
Added a second model to the excel file
</commit_message>
<xml_diff>
--- a/sqlResultCSVs/WinPercentVsMSU.xlsx
+++ b/sqlResultCSVs/WinPercentVsMSU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lissjust/Documents/NCAAWomens/sqlResultCSVs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C6AC4CB3-DAA1-B54F-B7FB-D74A2EBC591E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{10190F1E-B379-8A47-BB8C-3474DDDC53CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
@@ -909,7 +909,7 @@
   <dimension ref="A1:AH83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE9" sqref="AE9"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>